<commit_message>
Added target table too
</commit_message>
<xml_diff>
--- a/Level-II/Lecture3/mini project/data/table_metadata.xlsx
+++ b/Level-II/Lecture3/mini project/data/table_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\big_data_course\lecture9\mini project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kante\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D2817347-4B66-4847-BBA0-8E7256AB3AB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810C0EAE-8CA3-4143-B0A4-5BA6A11D7B44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Store" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Trans Codes" sheetId="6" r:id="rId6"/>
     <sheet name="Trans_Strings" sheetId="7" r:id="rId7"/>
     <sheet name="Trans String details" sheetId="8" r:id="rId8"/>
+    <sheet name="Target Table" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="235">
   <si>
     <t>Promo_code_id</t>
   </si>
@@ -720,6 +721,33 @@
   </si>
   <si>
     <t>Tacos/Fajita</t>
+  </si>
+  <si>
+    <t>Tx_Id</t>
+  </si>
+  <si>
+    <t>Store_Id</t>
+  </si>
+  <si>
+    <t>Product_Id</t>
+  </si>
+  <si>
+    <t>Loyalty_Member_Id</t>
+  </si>
+  <si>
+    <t>Promo_Code_Id</t>
+  </si>
+  <si>
+    <t>Emp_Id</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>Tx_Date</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1751,7 @@
   </sheetPr>
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -3550,7 +3578,7 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3836,4 +3864,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6C874D-B5B9-4712-A3F3-7169089D73DD}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>